<commit_message>
Tests changes for 3.0
</commit_message>
<xml_diff>
--- a/VC-performance-benchmark.xlsx
+++ b/VC-performance-benchmark.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VirtoCommerce\vc-benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9CA45B-7A8D-418C-AF93-E390206F65F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E74925-0B80-441E-8766-482F0E1F98D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report 2019 Benchmark (comp)" sheetId="9" r:id="rId1"/>
     <sheet name="Report 2019 Benchmark" sheetId="6" r:id="rId2"/>
-    <sheet name="3.0.0 - 2019 Baseline" sheetId="8" r:id="rId3"/>
-    <sheet name="2.49.0 - 2019 Baseline" sheetId="4" r:id="rId4"/>
-    <sheet name="Report 2017" sheetId="3" r:id="rId5"/>
-    <sheet name="B2 -2017" sheetId="1" r:id="rId6"/>
-    <sheet name="B3 - 2017" sheetId="2" r:id="rId7"/>
+    <sheet name="2.13.63 - 2020 Baseline" sheetId="11" r:id="rId3"/>
+    <sheet name="3.0.0 - 2020 Baseline" sheetId="10" r:id="rId4"/>
+    <sheet name="3.0.0-rc - 2019 Baseline" sheetId="8" r:id="rId5"/>
+    <sheet name="2.13.49 - 2019 Baseline" sheetId="4" r:id="rId6"/>
+    <sheet name="Report 2017" sheetId="3" r:id="rId7"/>
+    <sheet name="B2 -2017" sheetId="1" r:id="rId8"/>
+    <sheet name="B3 - 2017" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="70">
   <si>
     <t>Req/sec</t>
   </si>
@@ -377,6 +379,12 @@
   <si>
     <t>Start time</t>
   </si>
+  <si>
+    <t>Avg Req/sec</t>
+  </si>
+  <si>
+    <t>Max Users</t>
+  </si>
 </sst>
 </file>
 
@@ -467,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -490,15 +498,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -608,7 +617,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$A$11:$B$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$A$11:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -640,7 +649,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$D$11:$D$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$D$11:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -742,7 +751,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'3.0.0 - 2019 Baseline'!$D$11:$D$16</c:f>
+              <c:f>'3.0.0-rc - 2019 Baseline'!$D$11:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2447,7 +2456,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$A$11:$B$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$A$11:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2479,7 +2488,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$E$11:$E$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$E$11:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2581,7 +2590,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'3.0.0 - 2019 Baseline'!$E$11:$E$16</c:f>
+              <c:f>'3.0.0-rc - 2019 Baseline'!$E$11:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2906,7 +2915,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$A$11:$B$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$A$11:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2938,7 +2947,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$G$11:$G$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$G$11:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3000,7 +3009,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'3.0.0 - 2019 Baseline'!$G$11:$G$16</c:f>
+              <c:f>'3.0.0-rc - 2019 Baseline'!$G$11:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3281,7 +3290,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$E$17</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3293,7 +3302,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$E$17</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3380,7 +3389,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$E$17</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3392,7 +3401,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3.0.0 - 2019 Baseline'!$E$17</c:f>
+              <c:f>'3.0.0-rc - 2019 Baseline'!$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3721,7 +3730,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$A$3:$B$7</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$A$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3744,7 +3753,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$D$3:$D$7</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4017,7 +4026,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$A$3:$B$7</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$A$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4040,7 +4049,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$E$3:$E$7</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4311,7 +4320,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$A$11:$B$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$A$11:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4343,7 +4352,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$D$11:$D$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$D$11:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4609,7 +4618,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$A$11:$B$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$A$11:$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4641,7 +4650,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.49.0 - 2019 Baseline'!$E$11:$E$16</c:f>
+              <c:f>'2.13.49 - 2019 Baseline'!$E$11:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -8080,7 +8089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2795230-E63B-4D4D-B506-2043213D2641}">
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -8247,33 +8256,33 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="L15" s="17"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8285,7 +8294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7130AC16-F85C-4D9F-B504-80F44D6588AD}">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
@@ -8508,11 +8517,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0452D5-3C8A-4951-8B1C-279891977D1B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235B8700-4F2F-4515-9DD5-B3038D43B14B}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8585,10 +8594,10 @@
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="10"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -8616,129 +8625,115 @@
         <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="10">
-        <v>7360</v>
-      </c>
-      <c r="D11" s="2">
-        <v>41</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1.43</v>
+      <c r="C11" s="10"/>
+      <c r="D11" s="17">
+        <v>45.3</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1.23</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="10">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="10">
-        <v>59414</v>
-      </c>
+      <c r="C12" s="10"/>
       <c r="D12" s="2">
-        <v>198</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="E12" s="2">
-        <v>0.78</v>
+        <v>1.33</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="10">
-        <v>300</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="10">
-        <v>45180</v>
-      </c>
+      <c r="C13" s="10"/>
       <c r="D13" s="2">
-        <v>151</v>
+        <v>68</v>
       </c>
       <c r="E13" s="2">
-        <v>0.13</v>
+        <v>1.24</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="10">
-        <v>300</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="10">
-        <v>25836</v>
-      </c>
+      <c r="C14" s="10"/>
       <c r="D14" s="2">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2">
-        <v>1.28</v>
+        <v>1.25</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="10">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="10">
-        <v>846</v>
-      </c>
+      <c r="C15" s="10"/>
       <c r="D15" s="2">
-        <v>13.7</v>
+        <v>26.4</v>
       </c>
       <c r="E15" s="2">
-        <v>2.46</v>
+        <v>1.23</v>
       </c>
       <c r="G15" s="10">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="10">
-        <v>26643</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="2">
-        <v>82.1</v>
+        <v>21</v>
       </c>
       <c r="E16" s="2">
-        <v>1.58</v>
+        <v>2.13</v>
       </c>
       <c r="G16" s="10">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="10">
-        <v>15</v>
-      </c>
+      <c r="E17" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8751,11 +8746,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2E8872-4265-4342-AA08-30A9267778AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDEACA4-D9DD-47D9-852C-381272874DE7}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8798,87 +8793,44 @@
       <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="10">
-        <v>13979</v>
-      </c>
-      <c r="D3" s="2">
-        <v>46.6</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3.25</v>
-      </c>
-      <c r="G3">
-        <v>300</v>
-      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="10">
-        <v>23558</v>
-      </c>
-      <c r="D4" s="2">
-        <v>78.53</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.95</v>
-      </c>
-      <c r="G4">
-        <v>300</v>
-      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="11">
-        <v>37531</v>
-      </c>
-      <c r="D5" s="9">
-        <v>125</v>
-      </c>
-      <c r="E5" s="9">
-        <v>1.22</v>
-      </c>
-      <c r="G5">
-        <v>300</v>
-      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10">
-        <v>1938</v>
-      </c>
-      <c r="D6" s="2">
-        <v>6.46</v>
-      </c>
-      <c r="E6" s="2">
-        <v>20.73</v>
-      </c>
-      <c r="G6" s="12">
-        <v>170</v>
-      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="10">
-        <v>7038</v>
-      </c>
-      <c r="D7" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5.98</v>
-      </c>
-      <c r="G7" s="12">
-        <v>210</v>
-      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
@@ -8902,129 +8854,115 @@
         <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="10">
-        <v>15162</v>
-      </c>
-      <c r="D11" s="2">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2.1800000000000002</v>
+      <c r="C11" s="10"/>
+      <c r="D11" s="17">
+        <v>35</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1.58</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="10">
-        <v>300</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="10">
-        <v>24300</v>
-      </c>
+      <c r="C12" s="10"/>
       <c r="D12" s="2">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2">
-        <v>1.2</v>
+        <v>1.75</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="10">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="10">
-        <v>23406</v>
-      </c>
+      <c r="C13" s="10"/>
       <c r="D13" s="2">
-        <v>78</v>
+        <v>60.6</v>
       </c>
       <c r="E13" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.68</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="10">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="10">
-        <v>6125</v>
-      </c>
+      <c r="C14" s="10"/>
       <c r="D14" s="2">
-        <v>20.420000000000002</v>
+        <v>27.8</v>
       </c>
       <c r="E14" s="2">
-        <v>1.8</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="10">
-        <v>120</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="10">
-        <v>2100</v>
-      </c>
+      <c r="C15" s="10"/>
       <c r="D15" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G15" s="16">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="G15" s="10">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="10">
-        <v>23414</v>
-      </c>
+      <c r="A16" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="2">
-        <v>78.05</v>
+        <v>24.1</v>
       </c>
       <c r="E16" s="2">
-        <v>1.62</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="G16" s="10">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="10">
-        <v>35</v>
-      </c>
+      <c r="E17" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9037,10 +8975,539 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0452D5-3C8A-4951-8B1C-279891977D1B}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="10">
+        <v>7360</v>
+      </c>
+      <c r="D11" s="2">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.43</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="10">
+        <v>59414</v>
+      </c>
+      <c r="D12" s="2">
+        <v>198</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="10">
+        <v>45180</v>
+      </c>
+      <c r="D13" s="2">
+        <v>151</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="10">
+        <v>25836</v>
+      </c>
+      <c r="D14" s="2">
+        <v>91</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="10">
+        <v>846</v>
+      </c>
+      <c r="D15" s="2">
+        <v>13.7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.46</v>
+      </c>
+      <c r="G15" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="10">
+        <v>26643</v>
+      </c>
+      <c r="D16" s="2">
+        <v>82.1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.58</v>
+      </c>
+      <c r="G16" s="10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="10">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2E8872-4265-4342-AA08-30A9267778AC}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10">
+        <v>13979</v>
+      </c>
+      <c r="D3" s="2">
+        <v>46.6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="G3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="10">
+        <v>23558</v>
+      </c>
+      <c r="D4" s="2">
+        <v>78.53</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="G4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="11">
+        <v>37531</v>
+      </c>
+      <c r="D5" s="9">
+        <v>125</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1.22</v>
+      </c>
+      <c r="G5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1938</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.46</v>
+      </c>
+      <c r="E6" s="2">
+        <v>20.73</v>
+      </c>
+      <c r="G6" s="12">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="10">
+        <v>7038</v>
+      </c>
+      <c r="D7" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.98</v>
+      </c>
+      <c r="G7" s="12">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="10">
+        <v>15162</v>
+      </c>
+      <c r="D11" s="2">
+        <v>50</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="10">
+        <v>24300</v>
+      </c>
+      <c r="D12" s="2">
+        <v>150</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="10">
+        <v>23406</v>
+      </c>
+      <c r="D13" s="2">
+        <v>78</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="10">
+        <v>6125</v>
+      </c>
+      <c r="D14" s="2">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2100</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G15" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="10">
+        <v>23414</v>
+      </c>
+      <c r="D16" s="2">
+        <v>78.05</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="G16" s="10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="10">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -9268,12 +9735,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D12" sqref="D12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9368,10 +9835,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="10">
         <v>658</v>
       </c>
@@ -9478,10 +9945,10 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="14"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="10">
         <v>1067</v>
       </c>
@@ -9539,12 +10006,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E25:E26"/>
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9639,10 +10106,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="10">
         <v>1067</v>
       </c>
@@ -9749,10 +10216,10 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="14"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="10">
         <v>7040</v>
       </c>

</xml_diff>